<commit_message>
made changes to string handler
</commit_message>
<xml_diff>
--- a/Seasons.xlsx
+++ b/Seasons.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bala/Desktop/Curtin/1 Year/Sem2/ISEC/Final Assignment/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{40586AE4-90A1-4F4B-806A-1FC068D88FA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC9B5105-E0F1-174C-8A1B-60A1DBE5711A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19200" yWindow="0" windowWidth="19200" windowHeight="21600" xr2:uid="{08F3A871-05BE-E54B-8DE3-716121A63EDB}"/>
+    <workbookView xWindow="34400" yWindow="0" windowWidth="34400" windowHeight="28800" xr2:uid="{08F3A871-05BE-E54B-8DE3-716121A63EDB}"/>
   </bookViews>
   <sheets>
     <sheet name="Seasons" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="34">
   <si>
     <t xml:space="preserve">Country </t>
   </si>
@@ -114,6 +114,30 @@
   </si>
   <si>
     <t>Southeast Monsoon</t>
+  </si>
+  <si>
+    <t>Summer-Birak</t>
+  </si>
+  <si>
+    <t>Summer-Bunuru</t>
+  </si>
+  <si>
+    <t>Autumn-Bunuru</t>
+  </si>
+  <si>
+    <t>Autumn-Djeran</t>
+  </si>
+  <si>
+    <t>Winter-Makuru</t>
+  </si>
+  <si>
+    <t>Winter-Dijiba</t>
+  </si>
+  <si>
+    <t>Spring-Dijiba</t>
+  </si>
+  <si>
+    <t>Spring-Kambarang</t>
   </si>
 </sst>
 </file>
@@ -474,7 +498,7 @@
   <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -530,40 +554,40 @@
         <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="C2" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="D2" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="E2" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="F2" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="G2" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="H2" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="I2" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="J2" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="K2" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="L2" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="M2" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">

</xml_diff>